<commit_message>
Add interactive console output XML file with initial test results
- Created a new XML file for the Robot Interactive Console output.
- Included details of the default task/test execution with a PASS status.
- Added statistics summarizing the test results.
- Logged a warning regarding the use of deprecated singular section headers in the test case definition.
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/Login.xlsx
+++ b/ProjectTest65/Excel/Login.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59150221-1BB9-4ABF-AC93-4806FDC532B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="2688" yWindow="540" windowWidth="16908" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Login"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
   <si>
     <t>Execute</t>
   </si>
@@ -40,21 +46,21 @@
     <t>Revise</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>mju6204106317@mju.ac.th</t>
+  </si>
+  <si>
+    <t>เข้าสู่ระบบสำเร็จ</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>mju6204106317@mju.ac.th</t>
-  </si>
-  <si>
-    <t>บันทึกข้อมูลสำเร็จ</t>
-  </si>
-  <si>
-    <t>เข้าสู่ระบบสำเร็จ</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Siraprapha005@mju.ac.th</t>
   </si>
   <si>
@@ -80,9 +86,6 @@
   </si>
   <si>
     <t>ท่านยังไม่ได้รับการอนุมัติ</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>กรุณากรอกข้อมูลอีเมล</t>
@@ -100,8 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,13 +114,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -131,20 +133,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFee0000"/>
+      <color rgb="FFEE0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
@@ -158,7 +160,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFee0000"/>
+        <fgColor rgb="FFEE0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,16 +181,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -196,71 +198,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -271,10 +267,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -312,71 +308,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,7 +400,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -427,11 +423,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -440,13 +436,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -456,7 +452,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -465,7 +461,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -474,7 +470,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -482,10 +478,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -550,27 +546,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="F2:H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="14" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="25.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="38.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="38.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="38.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,72 +585,65 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="4">
         <v>111111</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="F2"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>111111</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>111111</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -663,22 +652,21 @@
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>111111</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -687,22 +675,21 @@
       <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>111111</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -711,22 +698,21 @@
       <c r="F6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>7</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>111111</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -735,22 +721,21 @@
       <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -759,102 +744,97 @@
       <c r="F8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
         <v>9</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="6">
+      <c r="C9" s="9"/>
+      <c r="D9" s="4">
         <v>111111</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    </row>
+    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>111111</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    </row>
+    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <v>123456</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>12</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="5" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: clean up code structure and remove redundant code blocks
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/Login.xlsx
+++ b/ProjectTest65/Excel/Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59150221-1BB9-4ABF-AC93-4806FDC532B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7294A9-FE15-420F-9A53-39BE03DE6B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="540" windowWidth="16908" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
   <si>
     <t>Execute</t>
   </si>
@@ -46,27 +46,33 @@
     <t>Revise</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>mju6204106317@mju.ac.th</t>
+  </si>
+  <si>
+    <t>เข้าสู่ระบบสำเร็จ</t>
+  </si>
+  <si>
+    <t>No message found</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>mju6204106317@mju.ac.th</t>
-  </si>
-  <si>
-    <t>เข้าสู่ระบบสำเร็จ</t>
+    <t>Siraprapha005@mju.ac.th</t>
+  </si>
+  <si>
+    <t>Email หรือ Passwordไม่ถูกต้อง กรุณาลองใหม่อีกครั้ง</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Siraprapha005@mju.ac.th</t>
-  </si>
-  <si>
-    <t>Email หรือ Passwordไม่ถูกต้อง กรุณาลองใหม่อีกครั้ง</t>
-  </si>
-  <si>
     <t>mju6204106317@gmail.com</t>
   </si>
   <si>
@@ -92,9 +98,6 @@
   </si>
   <si>
     <t>Please fill out this field.</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>กรุณากรอกรหัสผ่าน</t>
@@ -196,53 +199,53 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -552,8 +555,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="F2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,8 +564,8 @@
     <col min="1" max="1" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="38.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="44.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,149 +611,154 @@
       <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2"/>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4">
         <v>111111</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4">
         <v>111111</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4">
         <v>111111</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>6</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4">
         <v>111111</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4">
         <v>111111</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>8</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>9</v>
@@ -760,18 +768,18 @@
         <v>111111</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>10</v>
@@ -785,16 +793,16 @@
       <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
+      <c r="F10" t="s">
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>11</v>
@@ -806,18 +814,18 @@
         <v>123456</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>12</v>
@@ -827,13 +835,13 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test suite output and statistics in report.html
- Changed suite identifier from 68329 to 193889.
- Updated test case from registerTest to editProfileTest.
- Adjusted elapsed time for all tests from 00:01:07 to 00:03:13.
- Modified generated report size from 68512 to 194040.
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/Login.xlsx
+++ b/ProjectTest65/Excel/Login.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3B01C1-4FD0-415A-A5D9-9AC4334CF901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CA4DC6-3DF7-45A4-8C98-AF2ECB5C7BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
   <si>
     <t>Execute</t>
   </si>
@@ -92,18 +105,32 @@
   </si>
   <si>
     <t>กรุณากรอกรหัสผ่าน</t>
+  </si>
+  <si>
+    <t>สรุปผลการทดสอบ</t>
+  </si>
+  <si>
+    <t>คิดเป็น %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,8 +171,24 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +198,28 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEE0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -189,26 +254,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -218,13 +284,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,8 +308,30 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="4" builtinId="36"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,23 +635,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="44.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="44.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,14 +671,14 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="20.25" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -605,16 +697,19 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="20.25" customHeight="1">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>12</v>
@@ -628,16 +723,19 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="20.25" customHeight="1">
       <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>14</v>
@@ -651,16 +749,24 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" spans="1:13" ht="20.25" customHeight="1">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
@@ -674,16 +780,26 @@
       <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="20.25" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
@@ -697,16 +813,30 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="17">
+        <f>COUNTIF(G:G,"Pass")</f>
+        <v>9</v>
+      </c>
+      <c r="M6" s="17" t="str">
+        <f>TEXT(L6/11,"0.00%")</f>
+        <v>81.82%</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="20.25" customHeight="1">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>17</v>
@@ -720,16 +850,30 @@
       <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="18">
+        <f>COUNTIF(G:G,"Fail")</f>
+        <v>2</v>
+      </c>
+      <c r="M7" s="18" t="str">
+        <f>TEXT(L7/11,"0.00%")</f>
+        <v>18.18%</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="20.25" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>18</v>
@@ -743,16 +887,22 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="1:13" ht="20.25" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="4">
@@ -764,16 +914,22 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" spans="1:13" ht="20.25" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>9</v>
@@ -787,16 +943,24 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+    </row>
+    <row r="11" spans="1:13" ht="20.25" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
@@ -810,16 +974,26 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="23"/>
+      <c r="M11" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.25" customHeight="1">
       <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
@@ -831,11 +1005,44 @@
       <c r="F12" t="s">
         <v>21</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="H12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="17">
+        <f>COUNTIF(H:H,"Pass")</f>
+        <v>9</v>
+      </c>
+      <c r="M12" s="17" t="str">
+        <f>TEXT(L12/11,"0.00%")</f>
+        <v>81.82%</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="K13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="18">
+        <f>COUNTIF(H:H,"Fail")</f>
+        <v>2</v>
+      </c>
+      <c r="M13" s="18" t="str">
+        <f>TEXT(L13/11,"0.00%")</f>
+        <v>18.18%</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K11:L11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>